<commit_message>
project finished version 1.0
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -366,1445 +366,1448 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="12.88671875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
         <v>0.114879883126679</v>
       </c>
-      <c r="C2">
-        <v>1100.42</v>
+      <c r="C2" s="1">
+        <v>1.1004200000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3">
+    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
         <v>0.13079672909552301</v>
       </c>
-      <c r="C3">
-        <v>588.35</v>
+      <c r="C3" s="1">
+        <v>0.58835000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
         <v>0.116158493553509</v>
       </c>
-      <c r="C4">
-        <v>1281.23</v>
+      <c r="C4" s="1">
+        <v>1.2812300000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5">
+    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
         <v>0.13151665198896501</v>
       </c>
-      <c r="C5">
-        <v>1520.81</v>
+      <c r="C5" s="1">
+        <v>1.52081</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6">
+    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
         <v>0.13087135819589299</v>
       </c>
-      <c r="C6">
-        <v>2029.85</v>
+      <c r="C6" s="1">
+        <v>2.0298499999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
         <v>0.123411896998255</v>
       </c>
-      <c r="C7">
-        <v>6233.03</v>
+      <c r="C7" s="1">
+        <v>6.2330299999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
         <v>0.12458114779913899</v>
       </c>
-      <c r="C8">
-        <v>811.5</v>
+      <c r="C8" s="1">
+        <v>0.8115</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
         <v>0.116726199317854</v>
       </c>
-      <c r="C9">
-        <v>2706.07</v>
+      <c r="C9" s="1">
+        <v>2.70607</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
         <v>0.12473255478044699</v>
       </c>
-      <c r="C10">
-        <v>1449.61</v>
+      <c r="C10" s="1">
+        <v>1.4496099999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
         <v>0.11909733178481501</v>
       </c>
-      <c r="C11">
-        <v>3599.94</v>
+      <c r="C11" s="1">
+        <v>3.5999400000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
         <v>0.12275672628081</v>
       </c>
-      <c r="C12">
-        <v>1559.66</v>
+      <c r="C12" s="1">
+        <v>1.55966</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13">
+    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
         <v>0.11352430739471001</v>
       </c>
-      <c r="C13">
-        <v>1276.97</v>
+      <c r="C13" s="1">
+        <v>1.2769699999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14">
+    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
         <v>0.14137202924469</v>
       </c>
-      <c r="C14">
-        <v>695.06</v>
+      <c r="C14" s="1">
+        <v>0.6950599999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15">
+    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
         <v>0.120176306413682</v>
       </c>
-      <c r="C15">
-        <v>1084.54</v>
+      <c r="C15" s="1">
+        <v>1.0845400000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16">
+    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
         <v>0.109719665709993</v>
       </c>
-      <c r="C16">
-        <v>2330.73</v>
+      <c r="C16" s="1">
+        <v>2.33073</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17">
+    <row r="17" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
         <v>0.105445924767353</v>
       </c>
-      <c r="C17">
-        <v>33.31</v>
+      <c r="C17" s="1">
+        <v>3.3309999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18">
+    <row r="18" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
         <v>0.121499936247405</v>
       </c>
-      <c r="C18">
-        <v>286.62</v>
+      <c r="C18" s="1">
+        <v>0.28661999999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19">
+    <row r="19" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
         <v>0.123048681713048</v>
       </c>
-      <c r="C19">
-        <v>1864.19</v>
+      <c r="C19" s="1">
+        <v>1.86419</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20">
+    <row r="20" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
         <v>0.11903131293751899</v>
       </c>
-      <c r="C20">
-        <v>126.68</v>
+      <c r="C20" s="1">
+        <v>0.12668000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21">
+    <row r="21" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
         <v>0.10815124004641501</v>
       </c>
-      <c r="C21">
-        <v>552.78</v>
+      <c r="C21" s="1">
+        <v>0.55277999999999994</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22">
+    <row r="22" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
         <v>0.107689983705144</v>
       </c>
-      <c r="C22">
-        <v>153.76</v>
+      <c r="C22" s="1">
+        <v>0.15375999999999998</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23">
+    <row r="23" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
         <v>0.110788089343814</v>
       </c>
-      <c r="C23">
-        <v>607.28</v>
+      <c r="C23" s="1">
+        <v>0.60727999999999993</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24">
+    <row r="24" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
         <v>0.113637428728267</v>
       </c>
-      <c r="C24">
-        <v>203.3</v>
+      <c r="C24" s="1">
+        <v>0.20330000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25">
+    <row r="25" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
         <v>0.114553164455162</v>
       </c>
-      <c r="C25">
-        <v>2319.5100000000002</v>
+      <c r="C25" s="1">
+        <v>2.3195100000000002</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26">
+    <row r="26" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
         <v>0.122286994638805</v>
       </c>
-      <c r="C26">
-        <v>1186.95</v>
+      <c r="C26" s="1">
+        <v>1.1869499999999999</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27">
+    <row r="27" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
         <v>0.122979033920294</v>
       </c>
-      <c r="C27">
-        <v>409.11</v>
+      <c r="C27" s="1">
+        <v>0.40911000000000003</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28">
+    <row r="28" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
         <v>0.12164882065480299</v>
       </c>
-      <c r="C28">
-        <v>239.77</v>
+      <c r="C28" s="1">
+        <v>0.23977000000000001</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29">
+    <row r="29" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
         <v>0.11279770872809899</v>
       </c>
-      <c r="C29">
-        <v>534.04</v>
+      <c r="C29" s="1">
+        <v>0.53403999999999996</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30">
+    <row r="30" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
         <v>0.12768093179488699</v>
       </c>
-      <c r="C30">
-        <v>681.86</v>
+      <c r="C30" s="1">
+        <v>0.68186000000000002</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31">
+    <row r="31" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
         <v>0.136887614974979</v>
       </c>
-      <c r="C31">
-        <v>350.36</v>
+      <c r="C31" s="1">
+        <v>0.35036</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32">
+    <row r="32" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
         <v>0.13162915866456601</v>
       </c>
-      <c r="C32">
-        <v>386.01</v>
+      <c r="C32" s="1">
+        <v>0.38600999999999996</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33">
+    <row r="33" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
         <v>0.123422148118411</v>
       </c>
-      <c r="C33">
-        <v>526.14</v>
+      <c r="C33" s="1">
+        <v>0.52613999999999994</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34">
+    <row r="34" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
         <v>0.132832180022847</v>
       </c>
-      <c r="C34">
-        <v>2398.84</v>
+      <c r="C34" s="1">
+        <v>2.3988400000000003</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35">
+    <row r="35" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
         <v>0.138003256422329</v>
       </c>
-      <c r="C35">
-        <v>636.20000000000005</v>
+      <c r="C35" s="1">
+        <v>0.6362000000000001</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36">
+    <row r="36" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
         <v>0.11311889294056</v>
       </c>
-      <c r="C36">
-        <v>229.34</v>
+      <c r="C36" s="1">
+        <v>0.22934000000000002</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37">
+    <row r="37" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
         <v>0.131209533043947</v>
       </c>
-      <c r="C37">
-        <v>736.43</v>
+      <c r="C37" s="1">
+        <v>0.73642999999999992</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38">
+    <row r="38" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
         <v>0.13812334796428</v>
       </c>
-      <c r="C38">
-        <v>1148.42</v>
+      <c r="C38" s="1">
+        <v>1.14842</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39">
+    <row r="39" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
         <v>0.126823242301809</v>
       </c>
-      <c r="C39">
-        <v>1417.12</v>
+      <c r="C39" s="1">
+        <v>1.4171199999999999</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40">
+    <row r="40" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
         <v>0.14093102180073</v>
       </c>
-      <c r="C40">
-        <v>939.39</v>
+      <c r="C40" s="1">
+        <v>0.93938999999999995</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41">
+    <row r="41" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
         <v>0.131183287442901</v>
       </c>
-      <c r="C41">
-        <v>430.7</v>
+      <c r="C41" s="1">
+        <v>0.43069999999999997</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42">
+    <row r="42" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
         <v>0.116267422032848</v>
       </c>
-      <c r="C42">
-        <v>203.91</v>
+      <c r="C42" s="1">
+        <v>0.20391000000000001</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43">
+    <row r="43" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
         <v>0.10656434822472199</v>
       </c>
-      <c r="C43">
-        <v>107.23</v>
+      <c r="C43" s="1">
+        <v>0.10723000000000001</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44">
+    <row r="44" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
         <v>9.3544124596463996E-2</v>
       </c>
-      <c r="C44">
-        <v>227.48</v>
+      <c r="C44" s="1">
+        <v>0.22747999999999999</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45">
+    <row r="45" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
         <v>0.12619423510062799</v>
       </c>
-      <c r="C45">
-        <v>663.08</v>
+      <c r="C45" s="1">
+        <v>0.66308</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46">
+    <row r="46" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
         <v>0.11522457374372699</v>
       </c>
-      <c r="C46">
-        <v>31.65</v>
+      <c r="C46" s="1">
+        <v>3.1649999999999998E-2</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47">
+    <row r="47" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
         <v>0.12936032704223699</v>
       </c>
-      <c r="C47">
-        <v>605.29999999999995</v>
+      <c r="C47" s="1">
+        <v>0.60529999999999995</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48">
+    <row r="48" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
         <v>0.115152623358641</v>
       </c>
-      <c r="C48">
-        <v>339.04</v>
+      <c r="C48" s="1">
+        <v>0.33904000000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49">
+    <row r="49" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
         <v>0.103352029334095</v>
       </c>
-      <c r="C49">
-        <v>634.36</v>
+      <c r="C49" s="1">
+        <v>0.63436000000000003</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50">
+    <row r="50" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="1">
         <v>0.120403678603463</v>
       </c>
-      <c r="C50">
-        <v>221.92</v>
+      <c r="C50" s="1">
+        <v>0.22191999999999998</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51">
+    <row r="51" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="1">
         <v>0.105687656455726</v>
       </c>
-      <c r="C51">
-        <v>767.52</v>
+      <c r="C51" s="1">
+        <v>0.76751999999999998</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52">
+    <row r="52" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
         <v>0.12588283175918799</v>
       </c>
-      <c r="C52">
-        <v>151.91999999999999</v>
+      <c r="C52" s="1">
+        <v>0.15192</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53">
+    <row r="53" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="1">
         <v>0.12520254584445001</v>
       </c>
-      <c r="C53">
-        <v>496.57</v>
+      <c r="C53" s="1">
+        <v>0.49657000000000001</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54">
+    <row r="54" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
         <v>0.112784829910796</v>
       </c>
-      <c r="C54">
-        <v>744.13</v>
+      <c r="C54" s="1">
+        <v>0.74412999999999996</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55">
+    <row r="55" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
         <v>0.121271416068873</v>
       </c>
-      <c r="C55">
-        <v>159.09</v>
+      <c r="C55" s="1">
+        <v>0.15909000000000001</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56">
+    <row r="56" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="1">
         <v>0.107553961795992</v>
       </c>
-      <c r="C56">
-        <v>429.38</v>
+      <c r="C56" s="1">
+        <v>0.42937999999999998</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57">
+    <row r="57" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="1">
         <v>0.118876594381113</v>
       </c>
-      <c r="C57">
-        <v>2021.74</v>
+      <c r="C57" s="1">
+        <v>2.0217399999999999</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58">
+    <row r="58" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="1">
         <v>0.114597722372538</v>
       </c>
-      <c r="C58">
-        <v>4653.4799999999996</v>
+      <c r="C58" s="1">
+        <v>4.6534799999999992</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59">
+    <row r="59" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="1">
         <v>0.107791936404338</v>
       </c>
-      <c r="C59">
-        <v>76.22</v>
+      <c r="C59" s="1">
+        <v>7.6219999999999996E-2</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60">
+    <row r="60" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="1">
         <v>0.12701979736782201</v>
       </c>
-      <c r="C60">
-        <v>299.66000000000003</v>
+      <c r="C60" s="1">
+        <v>0.29966000000000004</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61">
+    <row r="61" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="1">
         <v>0.124674816143185</v>
       </c>
-      <c r="C61">
-        <v>58.72</v>
+      <c r="C61" s="1">
+        <v>5.8720000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62">
+    <row r="62" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="1">
         <v>0.118748444018022</v>
       </c>
-      <c r="C62">
-        <v>1273.8699999999999</v>
+      <c r="C62" s="1">
+        <v>1.2738699999999998</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63">
+    <row r="63" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="1">
         <v>0.106794967294839</v>
       </c>
-      <c r="C63">
-        <v>12.32</v>
+      <c r="C63" s="1">
+        <v>1.2320000000000001E-2</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64">
+    <row r="64" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="1">
         <v>0.123974276786295</v>
       </c>
-      <c r="C64">
-        <v>1251.79</v>
+      <c r="C64" s="1">
+        <v>1.25179</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65">
+    <row r="65" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="1">
         <v>0.12053336410229901</v>
       </c>
-      <c r="C65">
-        <v>1496.82</v>
+      <c r="C65" s="1">
+        <v>1.49682</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66">
+    <row r="66" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="1">
         <v>0.121876459617602</v>
       </c>
-      <c r="C66">
-        <v>1956.22</v>
+      <c r="C66" s="1">
+        <v>1.9562200000000001</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67">
+    <row r="67" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="1">
         <v>0.14093102180073</v>
       </c>
-      <c r="C67">
-        <v>939.39</v>
+      <c r="C67" s="1">
+        <v>0.93938999999999995</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68">
+    <row r="68" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
         <v>0.142023044260606</v>
       </c>
-      <c r="C68">
-        <v>2373.7199999999998</v>
+      <c r="C68" s="1">
+        <v>2.3737199999999996</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69">
+    <row r="69" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="1">
         <v>0.12650443739424</v>
       </c>
-      <c r="C69">
-        <v>1984.67</v>
+      <c r="C69" s="1">
+        <v>1.9846700000000002</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70">
+    <row r="70" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
         <v>0.118585897397781</v>
       </c>
-      <c r="C70">
-        <v>430.67</v>
+      <c r="C70" s="1">
+        <v>0.43067</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71">
+    <row r="71" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="1">
         <v>0.13079672909552301</v>
       </c>
-      <c r="C71">
-        <v>588.35</v>
+      <c r="C71" s="1">
+        <v>0.58835000000000004</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72">
+    <row r="72" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="1">
         <v>0.116706132503735</v>
       </c>
-      <c r="C72">
-        <v>847.06</v>
+      <c r="C72" s="1">
+        <v>0.84705999999999992</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73">
+    <row r="73" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="1">
         <v>0.104899142059692</v>
       </c>
-      <c r="C73">
-        <v>1603.17</v>
+      <c r="C73" s="1">
+        <v>1.60317</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74">
+    <row r="74" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="1">
         <v>0.12730342621921301</v>
       </c>
-      <c r="C74">
-        <v>1297.3599999999999</v>
+      <c r="C74" s="1">
+        <v>1.2973599999999998</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75">
+    <row r="75" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="1">
         <v>0.14101422827238799</v>
       </c>
-      <c r="C75">
-        <v>668.7</v>
+      <c r="C75" s="1">
+        <v>0.66870000000000007</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76">
+    <row r="76" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="1">
         <v>0.13626489254049301</v>
       </c>
-      <c r="C76">
-        <v>188.72</v>
+      <c r="C76" s="1">
+        <v>0.18872</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77">
+    <row r="77" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="1">
         <v>0.11711355887673</v>
       </c>
-      <c r="C77">
-        <v>70.900000000000006</v>
+      <c r="C77" s="1">
+        <v>7.0900000000000005E-2</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78">
+    <row r="78" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="1">
         <v>0.109941550531336</v>
       </c>
-      <c r="C78">
-        <v>472.1</v>
+      <c r="C78" s="1">
+        <v>0.47210000000000002</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B79">
+    <row r="79" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="1">
         <v>0.11422145047780401</v>
       </c>
-      <c r="C79">
-        <v>1259.68</v>
+      <c r="C79" s="1">
+        <v>1.2596800000000001</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80">
+    <row r="80" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="1">
         <v>0.13836605178588501</v>
       </c>
-      <c r="C80">
-        <v>1051.26</v>
+      <c r="C80" s="1">
+        <v>1.0512600000000001</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81">
+    <row r="81" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="1">
         <v>0.130069295064624</v>
       </c>
-      <c r="C81">
-        <v>308.3</v>
+      <c r="C81" s="1">
+        <v>0.30830000000000002</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82">
+    <row r="82" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="1">
         <v>0.149699498151077</v>
       </c>
-      <c r="C82">
-        <v>3294.36</v>
+      <c r="C82" s="1">
+        <v>3.2943600000000002</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B83">
+    <row r="83" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="1">
         <v>0.120720462394518</v>
       </c>
-      <c r="C83">
-        <v>215.4</v>
+      <c r="C83" s="1">
+        <v>0.21540000000000001</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84">
+    <row r="84" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="1">
         <v>0.117752413654236</v>
       </c>
-      <c r="C84">
-        <v>960.05</v>
+      <c r="C84" s="1">
+        <v>0.96004999999999996</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85">
+    <row r="85" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="1">
         <v>0.12904577967644401</v>
       </c>
-      <c r="C85">
-        <v>1087.77</v>
+      <c r="C85" s="1">
+        <v>1.0877699999999999</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86">
+    <row r="86" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="1">
         <v>0.11432487608681</v>
       </c>
-      <c r="C86">
-        <v>828.07</v>
+      <c r="C86" s="1">
+        <v>0.82807000000000008</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B87">
+    <row r="87" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="1">
         <v>0.110861430139624</v>
       </c>
-      <c r="C87">
-        <v>5.17</v>
+      <c r="C87" s="1">
+        <v>5.1700000000000001E-3</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88">
+    <row r="88" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="1">
         <v>0.120003951624349</v>
       </c>
-      <c r="C88">
-        <v>1162.51</v>
+      <c r="C88" s="1">
+        <v>1.1625099999999999</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89">
+    <row r="89" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="1">
         <v>0.125181383222007</v>
       </c>
-      <c r="C89">
-        <v>1425.44</v>
+      <c r="C89" s="1">
+        <v>1.42544</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B90">
+    <row r="90" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="1">
         <v>0.10769059903327199</v>
       </c>
-      <c r="C90">
-        <v>3596.29</v>
+      <c r="C90" s="1">
+        <v>3.5962899999999998</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91">
+    <row r="91" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="1">
         <v>0.102359875732591</v>
       </c>
-      <c r="C91">
-        <v>6124.06</v>
+      <c r="C91" s="1">
+        <v>6.1240600000000001</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92">
+    <row r="92" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="1">
         <v>0.119006943072756</v>
       </c>
-      <c r="C92">
-        <v>629.29</v>
+      <c r="C92" s="1">
+        <v>0.62929000000000002</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93">
+    <row r="93" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="1">
         <v>0.12538044983136401</v>
       </c>
-      <c r="C93">
-        <v>469.46</v>
+      <c r="C93" s="1">
+        <v>0.46945999999999999</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94">
+    <row r="94" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="1">
         <v>0.10769059903327199</v>
       </c>
-      <c r="C94">
-        <v>3596.29</v>
+      <c r="C94" s="1">
+        <v>3.5962899999999998</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95">
+    <row r="95" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="1">
         <v>0.14158637969040699</v>
       </c>
-      <c r="C95">
-        <v>12.58</v>
+      <c r="C95" s="1">
+        <v>1.2580000000000001E-2</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96">
+    <row r="96" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="1">
         <v>0.10940777757230601</v>
       </c>
-      <c r="C96">
-        <v>2022.7</v>
+      <c r="C96" s="1">
+        <v>2.0226999999999999</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97">
+    <row r="97" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="1">
         <v>0.12577119820872501</v>
       </c>
-      <c r="C97">
-        <v>1111.1500000000001</v>
+      <c r="C97" s="1">
+        <v>1.1111500000000001</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98">
+    <row r="98" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="1">
         <v>0.12085566870497599</v>
       </c>
-      <c r="C98">
-        <v>654.73</v>
+      <c r="C98" s="1">
+        <v>0.65473000000000003</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99">
+    <row r="99" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="1">
         <v>0.14024439615751</v>
       </c>
-      <c r="C99">
-        <v>1153.82</v>
+      <c r="C99" s="1">
+        <v>1.1538199999999998</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100">
+    <row r="100" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="1">
         <v>0.111010781268716</v>
       </c>
-      <c r="C100">
-        <v>2722.87</v>
+      <c r="C100" s="1">
+        <v>2.7228699999999999</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101">
+    <row r="101" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="1">
         <v>0.11950175392017</v>
       </c>
-      <c r="C101">
-        <v>4469.29</v>
+      <c r="C101" s="1">
+        <v>4.46929</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102">
+    <row r="102" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="1">
         <v>0.114859032506387</v>
       </c>
-      <c r="C102">
-        <v>30.96</v>
+      <c r="C102" s="1">
+        <v>3.0960000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103">
+    <row r="103" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="1">
         <v>0.130833514421408</v>
       </c>
-      <c r="C103">
-        <v>716.32</v>
+      <c r="C103" s="1">
+        <v>0.71632000000000007</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104">
+    <row r="104" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="1">
         <v>0.15226650734013</v>
       </c>
-      <c r="C104">
-        <v>304.33999999999997</v>
+      <c r="C104" s="1">
+        <v>0.30434</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105">
+    <row r="105" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="1">
         <v>0.12067600831155301</v>
       </c>
-      <c r="C105">
-        <v>741.71</v>
+      <c r="C105" s="1">
+        <v>0.74171000000000009</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106">
+    <row r="106" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="1">
         <v>0.12164882065480299</v>
       </c>
-      <c r="C106">
-        <v>239.77</v>
+      <c r="C106" s="1">
+        <v>0.23977000000000001</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107">
+    <row r="107" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="1">
         <v>0.114879883126679</v>
       </c>
-      <c r="C107">
-        <v>1100.42</v>
+      <c r="C107" s="1">
+        <v>1.1004200000000002</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108">
+    <row r="108" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="1">
         <v>0.13241640477946001</v>
       </c>
-      <c r="C108">
-        <v>1111.1300000000001</v>
+      <c r="C108" s="1">
+        <v>1.1111300000000002</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B109">
+    <row r="109" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="1">
         <v>0.11900253139570099</v>
       </c>
-      <c r="C109">
-        <v>376.62</v>
+      <c r="C109" s="1">
+        <v>0.37662000000000001</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B110">
+    <row r="110" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="1">
         <v>0.112484963057842</v>
       </c>
-      <c r="C110">
-        <v>1150.18</v>
+      <c r="C110" s="1">
+        <v>1.15018</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B111">
+    <row r="111" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="1">
         <v>0.103747062147998</v>
       </c>
-      <c r="C111">
-        <v>896.18</v>
+      <c r="C111" s="1">
+        <v>0.89617999999999998</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B112">
+    <row r="112" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="1">
         <v>0.14725723182615999</v>
       </c>
-      <c r="C112">
-        <v>915.4</v>
+      <c r="C112" s="1">
+        <v>0.91539999999999999</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B113">
+    <row r="113" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="1">
         <v>0.11401495063202099</v>
       </c>
-      <c r="C113">
-        <v>765.7</v>
+      <c r="C113" s="1">
+        <v>0.76570000000000005</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B114">
+    <row r="114" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="1">
         <v>0.111288980663709</v>
       </c>
-      <c r="C114">
-        <v>754.35</v>
+      <c r="C114" s="1">
+        <v>0.75435000000000008</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B115">
+    <row r="115" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="1">
         <v>0.10188030095091601</v>
       </c>
-      <c r="C115">
-        <v>598.80999999999995</v>
+      <c r="C115" s="1">
+        <v>0.59880999999999995</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B116">
+    <row r="116" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="1">
         <v>0.111732831686035</v>
       </c>
-      <c r="C116">
-        <v>559.29</v>
+      <c r="C116" s="1">
+        <v>0.55928999999999995</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B117">
+    <row r="117" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="1">
         <v>0.125312478763623</v>
       </c>
-      <c r="C117">
-        <v>1929.15</v>
+      <c r="C117" s="1">
+        <v>1.9291500000000001</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B118">
+    <row r="118" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="1">
         <v>0.14024439615751</v>
       </c>
-      <c r="C118">
-        <v>1153.82</v>
+      <c r="C118" s="1">
+        <v>1.1538199999999998</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B119">
+    <row r="119" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="1">
         <v>0.115076118196488</v>
       </c>
-      <c r="C119">
-        <v>944.49</v>
+      <c r="C119" s="1">
+        <v>0.94449000000000005</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B120">
+    <row r="120" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="1">
         <v>0.123133354198898</v>
       </c>
-      <c r="C120">
-        <v>4260.17</v>
+      <c r="C120" s="1">
+        <v>4.2601700000000005</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B121">
+    <row r="121" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="1">
         <v>0.14180174371068499</v>
       </c>
-      <c r="C121">
-        <v>1103.71</v>
+      <c r="C121" s="1">
+        <v>1.10371</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B122">
+    <row r="122" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="1">
         <v>0.12544249993876899</v>
       </c>
-      <c r="C122">
-        <v>2135.25</v>
+      <c r="C122" s="1">
+        <v>2.1352500000000001</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B123">
+    <row r="123" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B123" s="1">
         <v>0.121385601505102</v>
       </c>
-      <c r="C123">
-        <v>1891.39</v>
+      <c r="C123" s="1">
+        <v>1.8913900000000001</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B124">
+    <row r="124" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="1">
         <v>0.127620745251878</v>
       </c>
-      <c r="C124">
-        <v>627.71</v>
+      <c r="C124" s="1">
+        <v>0.62770999999999999</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B125">
+    <row r="125" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="1">
         <v>0.119270415379718</v>
       </c>
-      <c r="C125">
-        <v>1979.27</v>
+      <c r="C125" s="1">
+        <v>1.9792700000000001</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B126">
+    <row r="126" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="1">
         <v>9.7552996159554706E-2</v>
       </c>
-      <c r="C126">
-        <v>563.58000000000004</v>
+      <c r="C126" s="1">
+        <v>0.56358000000000008</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B127">
+    <row r="127" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="1">
         <v>0.104507414183792</v>
       </c>
-      <c r="C127">
-        <v>1705.65</v>
+      <c r="C127" s="1">
+        <v>1.7056500000000001</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B128">
+    <row r="128" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="1">
         <v>0.139781555347993</v>
       </c>
-      <c r="C128">
-        <v>840.02</v>
+      <c r="C128" s="1">
+        <v>0.84001999999999999</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B129">
+    <row r="129" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="1">
         <v>0.126919329861821</v>
       </c>
-      <c r="C129">
-        <v>2306.5500000000002</v>
+      <c r="C129" s="1">
+        <v>2.3065500000000001</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B130">
+    <row r="130" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="1">
         <v>0.11568302034748899</v>
       </c>
-      <c r="C130">
-        <v>1810.44</v>
+      <c r="C130" s="1">
+        <v>1.81044</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B131">
+    <row r="131" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="1">
         <v>0.131899311931166</v>
       </c>
-      <c r="C131">
-        <v>4255.7299999999996</v>
+      <c r="C131" s="1">
+        <v>4.2557299999999998</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B132">
+    <row r="132" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="1">
         <v>0.12562341006587299</v>
       </c>
-      <c r="C132">
-        <v>36.909999999999997</v>
+      <c r="C132" s="1">
+        <v>3.6909999999999998E-2</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B133">
+    <row r="133" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="1">
         <v>0.118039208761997</v>
       </c>
-      <c r="C133">
-        <v>2330.2600000000002</v>
+      <c r="C133" s="1">
+        <v>2.33026</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B134">
+    <row r="134" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="1">
         <v>0.116473540974801</v>
       </c>
-      <c r="C134">
-        <v>2022.8</v>
+      <c r="C134" s="1">
+        <v>2.0228000000000002</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B135">
+    <row r="135" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="1">
         <v>0.12893106117064601</v>
       </c>
-      <c r="C135">
-        <v>530.38</v>
+      <c r="C135" s="1">
+        <v>0.53037999999999996</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B136">
+    <row r="136" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="1">
         <v>0.11889342052067001</v>
       </c>
-      <c r="C136">
-        <v>1674.26</v>
+      <c r="C136" s="1">
+        <v>1.6742600000000001</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B137">
+    <row r="137" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="1">
         <v>0.105831678396427</v>
       </c>
-      <c r="C137">
-        <v>776.81</v>
+      <c r="C137" s="1">
+        <v>0.77681</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B138">
+    <row r="138" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B138" s="1">
         <v>0.13008895975031901</v>
       </c>
-      <c r="C138">
-        <v>171.27</v>
+      <c r="C138" s="1">
+        <v>0.17127000000000001</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B139">
+    <row r="139" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="1">
         <v>0.117024984814526</v>
       </c>
-      <c r="C139">
-        <v>21.29</v>
+      <c r="C139" s="1">
+        <v>2.129E-2</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B140">
+    <row r="140" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="1">
         <v>0.122616715391762</v>
       </c>
-      <c r="C140">
-        <v>2073.44</v>
+      <c r="C140" s="1">
+        <v>2.0734400000000002</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B141">
+    <row r="141" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="1">
         <v>0.10597260436612101</v>
       </c>
-      <c r="C141">
-        <v>402.8</v>
+      <c r="C141" s="1">
+        <v>0.40279999999999999</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B142">
+    <row r="142" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="1">
         <v>0.114200693464015</v>
       </c>
-      <c r="C142">
-        <v>1985.78</v>
+      <c r="C142" s="1">
+        <v>1.9857799999999999</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B143">
+    <row r="143" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="1">
         <v>0.130052721310386</v>
       </c>
-      <c r="C143">
-        <v>1507.68</v>
+      <c r="C143" s="1">
+        <v>1.5076800000000001</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144">
+    <row r="144" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="1">
         <v>0.12502497999199699</v>
       </c>
-      <c r="C144">
-        <v>1402.55</v>
+      <c r="C144" s="1">
+        <v>1.40255</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B145">
+    <row r="145" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="1">
         <v>0.124017484343663</v>
       </c>
-      <c r="C145">
-        <v>1610.76</v>
+      <c r="C145" s="1">
+        <v>1.61076</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B146">
+    <row r="146" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="1">
         <v>0.120482585875008</v>
       </c>
-      <c r="C146">
-        <v>2822</v>
+      <c r="C146" s="1">
+        <v>2.8220000000000001</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B147">
+    <row r="147" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="1">
         <v>0.137283965062406</v>
       </c>
-      <c r="C147">
-        <v>1579.66</v>
+      <c r="C147" s="1">
+        <v>1.5796600000000001</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B148">
+    <row r="148" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="1">
         <v>0.110782903843092</v>
       </c>
-      <c r="C148">
-        <v>1632.9</v>
+      <c r="C148" s="1">
+        <v>1.6329</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B149">
+    <row r="149" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="1">
         <v>0.11575097492842</v>
       </c>
-      <c r="C149">
-        <v>888.89</v>
+      <c r="C149" s="1">
+        <v>0.88888999999999996</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B150">
+    <row r="150" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B150" s="1">
         <v>0.11100821630419</v>
       </c>
-      <c r="C150">
-        <v>821.15</v>
+      <c r="C150" s="1">
+        <v>0.82114999999999994</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B151">
+    <row r="151" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B151" s="1">
         <v>0.12313805384351401</v>
       </c>
-      <c r="C151">
-        <v>298.33999999999997</v>
+      <c r="C151" s="1">
+        <v>0.29833999999999999</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B152">
+    <row r="152" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="1">
         <v>0.10918742192327099</v>
       </c>
-      <c r="C152">
-        <v>1948.78</v>
+      <c r="C152" s="1">
+        <v>1.94878</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B153">
+    <row r="153" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="1">
         <v>0.113861040229192</v>
       </c>
-      <c r="C153">
-        <v>2308.89</v>
+      <c r="C153" s="1">
+        <v>2.3088899999999999</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B154">
+    <row r="154" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B154" s="1">
         <v>0.118997974195949</v>
       </c>
-      <c r="C154">
-        <v>1896.02</v>
+      <c r="C154" s="1">
+        <v>1.89602</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B155">
+    <row r="155" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B155" s="1">
         <v>0.122529811751396</v>
       </c>
-      <c r="C155">
-        <v>469.53</v>
+      <c r="C155" s="1">
+        <v>0.46952999999999995</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B156">
+    <row r="156" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="1">
         <v>0.139661030161608</v>
       </c>
-      <c r="C156">
-        <v>1061.44</v>
+      <c r="C156" s="1">
+        <v>1.0614400000000002</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B157">
+    <row r="157" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="1">
         <v>0.100034895177514</v>
       </c>
-      <c r="C157">
-        <v>1698.73</v>
+      <c r="C157" s="1">
+        <v>1.6987300000000001</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B158">
+    <row r="158" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="1">
         <v>0.122960509355634</v>
       </c>
-      <c r="C158">
-        <v>1525.36</v>
+      <c r="C158" s="1">
+        <v>1.5253599999999998</v>
       </c>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B159">
+    <row r="159" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="1">
         <v>0.111633192224839</v>
       </c>
-      <c r="C159">
-        <v>1539.45</v>
+      <c r="C159" s="1">
+        <v>1.53945</v>
       </c>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B160">
+    <row r="160" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="1">
         <v>0.16967772054637001</v>
       </c>
-      <c r="C160">
-        <v>1201.46</v>
+      <c r="C160" s="1">
+        <v>1.20146</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B161">
+    <row r="161" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="1">
         <v>0.110581160221942</v>
       </c>
-      <c r="C161">
-        <v>571.83000000000004</v>
+      <c r="C161" s="1">
+        <v>0.57183000000000006</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B162">
+    <row r="162" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B162" s="1">
         <v>0.12124847218594099</v>
       </c>
-      <c r="C162">
-        <v>1623.67</v>
+      <c r="C162" s="1">
+        <v>1.6236700000000002</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B163">
+    <row r="163" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="1">
         <v>0.117301805451674</v>
       </c>
-      <c r="C163">
-        <v>1991.17</v>
+      <c r="C163" s="1">
+        <v>1.9911700000000001</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B164">
+    <row r="164" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="1">
         <v>0.12442221620289499</v>
       </c>
-      <c r="C164">
-        <v>393.57</v>
+      <c r="C164" s="1">
+        <v>0.39356999999999998</v>
       </c>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B165">
+    <row r="165" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="1">
         <v>0.116147916802066</v>
       </c>
-      <c r="C165">
-        <v>268.14</v>
+      <c r="C165" s="1">
+        <v>0.26813999999999999</v>
       </c>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B166">
+    <row r="166" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="1">
         <v>0.11276951866392</v>
       </c>
-      <c r="C166">
-        <v>919.94</v>
+      <c r="C166" s="1">
+        <v>0.91994000000000009</v>
       </c>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B167">
+    <row r="167" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B167" s="1">
         <v>0.122381116908948</v>
       </c>
-      <c r="C167">
-        <v>1416.79</v>
+      <c r="C167" s="1">
+        <v>1.41679</v>
       </c>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B168">
+    <row r="168" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B168" s="1">
         <v>0.117288435573963</v>
       </c>
-      <c r="C168">
-        <v>1414.96</v>
+      <c r="C168" s="1">
+        <v>1.41496</v>
       </c>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B169">
+    <row r="169" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B169" s="1">
         <v>0.10806748999316799</v>
       </c>
-      <c r="C169">
-        <v>53.82</v>
+      <c r="C169" s="1">
+        <v>5.382E-2</v>
       </c>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B170">
+    <row r="170" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B170" s="1">
         <v>0.12890417585303299</v>
       </c>
-      <c r="C170">
-        <v>458.27</v>
+      <c r="C170" s="1">
+        <v>0.45826999999999996</v>
       </c>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B171">
+    <row r="171" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B171" s="1">
         <v>0.125027782710221</v>
       </c>
-      <c r="C171">
-        <v>840.48</v>
+      <c r="C171" s="1">
+        <v>0.84048</v>
       </c>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B172">
+    <row r="172" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B172" s="1">
         <v>0.11610177964407099</v>
       </c>
-      <c r="C172">
-        <v>713.43</v>
+      <c r="C172" s="1">
+        <v>0.7134299999999999</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B173">
+    <row r="173" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B173" s="1">
         <v>0.114842930401438</v>
       </c>
-      <c r="C173">
-        <v>1138.33</v>
+      <c r="C173" s="1">
+        <v>1.1383299999999998</v>
       </c>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B174">
+    <row r="174" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B174" s="1">
         <v>0.103546776422158</v>
       </c>
-      <c r="C174">
-        <v>619.78</v>
+      <c r="C174" s="1">
+        <v>0.61978</v>
       </c>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B175">
+    <row r="175" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B175" s="1">
         <v>9.75040072872492E-2</v>
       </c>
-      <c r="C175">
-        <v>1231.92</v>
+      <c r="C175" s="1">
+        <v>1.2319200000000001</v>
       </c>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B176">
+    <row r="176" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B176" s="1">
         <v>0.102677704237466</v>
       </c>
-      <c r="C176">
-        <v>2026.25</v>
+      <c r="C176" s="1">
+        <v>2.0262500000000001</v>
       </c>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B177">
+    <row r="177" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B177" s="1">
         <v>0.11339512207134</v>
       </c>
-      <c r="C177">
-        <v>1444.39</v>
+      <c r="C177" s="1">
+        <v>1.4443900000000001</v>
       </c>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B178">
+    <row r="178" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B178" s="1">
         <v>0.11793412106366701</v>
       </c>
-      <c r="C178">
-        <v>1712.34</v>
+      <c r="C178" s="1">
+        <v>1.71234</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1812,11 +1815,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DM178"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D176" sqref="D176"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:117" x14ac:dyDescent="0.25">
       <c r="A1" s="1">

</xml_diff>